<commit_message>
All string IDs changed to ints
</commit_message>
<xml_diff>
--- a/Other files/Prediction Period table formatting.xlsx
+++ b/Other files/Prediction Period table formatting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1312D5C-F08B-4BB6-B868-92D6BB14480F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8559F1C6-2F8E-4CDB-AA3B-63E567CC79D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00994BDA-137B-48B0-9BDA-FB6372B0FE43}"/>
   </bookViews>
@@ -143,26 +143,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,31 +510,31 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="8">
@@ -543,171 +543,171 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
@@ -746,11 +746,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="E2:E3"/>
@@ -759,6 +754,11 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
About to start improving predictions board
</commit_message>
<xml_diff>
--- a/Other files/Prediction Period table formatting.xlsx
+++ b/Other files/Prediction Period table formatting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TheQBCarousel\Other files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8559F1C6-2F8E-4CDB-AA3B-63E567CC79D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE821F5B-19AE-4A7D-990B-D95A5087C62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00994BDA-137B-48B0-9BDA-FB6372B0FE43}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="19">
   <si>
     <t>From
 To</t>
@@ -71,6 +71,30 @@
   </si>
   <si>
     <t>PP4</t>
+  </si>
+  <si>
+    <t>toEventRow1</t>
+  </si>
+  <si>
+    <t>toEventRow2</t>
+  </si>
+  <si>
+    <t>isFirstPP</t>
+  </si>
+  <si>
+    <t>isLastPP</t>
+  </si>
+  <si>
+    <t>imageRow</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>fromEventRow</t>
+  </si>
+  <si>
+    <t>ppRow</t>
   </si>
 </sst>
 </file>
@@ -155,14 +179,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A611AB-B4D0-4BAB-9489-CA806E8B9273}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,9 +514,10 @@
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -509,35 +534,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="10">
         <v>2023</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -546,143 +583,213 @@
       <c r="D4" s="4"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="1"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="1"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="1"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="1"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="1"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="1"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="1"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
-        <v>15</v>
-      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
       <c r="D16" s="7"/>
@@ -690,24 +797,20 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
-        <v>16</v>
-      </c>
+      <c r="A17" s="6"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
-        <v>17</v>
-      </c>
+      <c r="A18" s="6"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
@@ -746,6 +849,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="E2:E3"/>
@@ -754,11 +862,6 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>